<commit_message>
Products upload excel sheet updated
</commit_message>
<xml_diff>
--- a/docs/Products upload.xlsx
+++ b/docs/Products upload.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="48" windowWidth="16260" windowHeight="6888" tabRatio="491"/>
+    <workbookView xWindow="384" yWindow="48" windowWidth="16260" windowHeight="6888" tabRatio="491" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
   <si>
     <t>Company Id</t>
   </si>
@@ -156,24 +156,6 @@
     <t>White Gold Ring</t>
   </si>
   <si>
-    <t>Yellow Gold Ring</t>
-  </si>
-  <si>
-    <t>Silver Ring</t>
-  </si>
-  <si>
-    <t>Platinum</t>
-  </si>
-  <si>
-    <t>Pink Gold Ring</t>
-  </si>
-  <si>
-    <t>Gems Ring</t>
-  </si>
-  <si>
-    <t>Beads Ring</t>
-  </si>
-  <si>
     <t>Ring size</t>
   </si>
   <si>
@@ -265,6 +247,15 @@
   </si>
   <si>
     <t>Images: comma "," separated images link</t>
+  </si>
+  <si>
+    <t>Half Eternity Ring</t>
+  </si>
+  <si>
+    <t>Full Eternity Ring</t>
+  </si>
+  <si>
+    <t>Solitaire Ring</t>
   </si>
 </sst>
 </file>
@@ -765,7 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -801,7 +792,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -846,10 +837,10 @@
         <v>41</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="T1" s="17" t="s">
         <v>38</v>
@@ -863,7 +854,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>44</v>
@@ -884,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="K2" s="3">
         <v>1</v>
@@ -911,10 +902,10 @@
         <v>50</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="T2" s="18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -1007,33 +998,33 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="T14" s="20"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -1041,13 +1032,13 @@
     </row>
     <row r="17" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="T17" s="20"/>
     </row>
     <row r="18" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -1057,7 +1048,7 @@
     </row>
     <row r="19" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -1067,7 +1058,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
@@ -1076,23 +1067,23 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B21" s="22"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -1122,7 +1113,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1130,7 +1121,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1138,7 +1129,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1146,7 +1137,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1154,7 +1145,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1162,7 +1153,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1188,7 +1179,7 @@
         <v>19</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1196,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1204,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1212,7 +1203,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1456,15 +1447,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1488,7 +1479,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1496,47 +1487,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
-        <v>5</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
-        <v>7</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
-        <v>8</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>46</v>
+      <c r="B5" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added "amount" column to Products upload excel sheet.
</commit_message>
<xml_diff>
--- a/docs/Products upload.xlsx
+++ b/docs/Products upload.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="48" windowWidth="16260" windowHeight="6888" tabRatio="491" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="384" yWindow="48" windowWidth="16260" windowHeight="6888" tabRatio="491"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="81">
   <si>
     <t>Company Id</t>
   </si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t>Solitaire Ring</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Amount: In Euros</t>
   </si>
 </sst>
 </file>
@@ -754,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,25 +772,26 @@
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="57.5546875" style="20" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="57.5546875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -798,55 +805,58 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -860,55 +870,58 @@
         <v>44</v>
       </c>
       <c r="E2" s="3">
+        <v>100</v>
+      </c>
+      <c r="F2" s="3">
         <v>10</v>
       </c>
-      <c r="F2" s="16">
+      <c r="G2" s="16">
         <v>15</v>
       </c>
-      <c r="G2" s="16">
+      <c r="H2" s="16">
         <v>1.2</v>
       </c>
-      <c r="H2" s="16">
+      <c r="I2" s="16">
         <v>5</v>
       </c>
-      <c r="I2" s="16">
+      <c r="J2" s="16">
         <v>1</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>1</v>
       </c>
-      <c r="L2" s="16">
+      <c r="M2" s="16">
         <v>1</v>
       </c>
-      <c r="M2" s="16">
+      <c r="N2" s="16">
         <v>10</v>
       </c>
-      <c r="N2" s="16">
+      <c r="O2" s="16">
         <v>20</v>
       </c>
-      <c r="O2" s="16">
+      <c r="P2" s="16">
         <v>10</v>
-      </c>
-      <c r="P2" s="3">
-        <v>4</v>
       </c>
       <c r="Q2" s="3">
         <v>4</v>
       </c>
       <c r="R2" s="3">
+        <v>4</v>
+      </c>
+      <c r="S2" s="3">
         <v>50</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="T2" s="18" t="s">
+      <c r="U2" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -928,9 +941,10 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="18"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T3" s="3"/>
+      <c r="U3" s="18"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -950,9 +964,10 @@
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
-      <c r="T4" s="18"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T4" s="3"/>
+      <c r="U4" s="18"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -972,9 +987,10 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
-      <c r="T5" s="18"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T5" s="3"/>
+      <c r="U5" s="18"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -994,100 +1010,112 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="19"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T6" s="1"/>
+      <c r="U6" s="19"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="T14" s="20"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="U14" s="20"/>
+    </row>
+    <row r="15" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U15" s="20"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-    </row>
-    <row r="17" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T17" s="20"/>
-    </row>
-    <row r="18" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+      <c r="U18" s="20"/>
+    </row>
+    <row r="19" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="T18" s="20"/>
-    </row>
-    <row r="19" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
-        <v>69</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
-      <c r="T19" s="20"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F19" s="21"/>
+      <c r="U19" s="20"/>
+    </row>
+    <row r="20" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="F20" s="21"/>
+      <c r="U20" s="20"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="22"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="B22" s="22"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A26" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1449,7 +1477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Products upload excel sheet - added discount percentage
</commit_message>
<xml_diff>
--- a/docs/Products upload.xlsx
+++ b/docs/Products upload.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
   <si>
     <t>Company Id</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>Amount: In Euros</t>
+  </si>
+  <si>
+    <t>Discount Percent</t>
+  </si>
+  <si>
+    <t>Discount Percent: If this is filled, then item will be shown as sale item and price would be calculated as (Amount - discount%) + VAT%, i.e. in Above case, (100 - 20) + 16.8 = 96.8 euros</t>
   </si>
 </sst>
 </file>
@@ -760,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,25 +779,26 @@
     <col min="3" max="3" width="10.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="57.5546875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="57.5546875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -808,55 +815,58 @@
         <v>79</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -872,56 +882,59 @@
       <c r="E2" s="3">
         <v>100</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="16">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3">
         <v>10</v>
       </c>
-      <c r="G2" s="16">
+      <c r="H2" s="16">
         <v>15</v>
       </c>
-      <c r="H2" s="16">
+      <c r="I2" s="16">
         <v>1.2</v>
       </c>
-      <c r="I2" s="16">
+      <c r="J2" s="16">
         <v>5</v>
       </c>
-      <c r="J2" s="16">
+      <c r="K2" s="16">
         <v>1</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="3">
         <v>1</v>
       </c>
-      <c r="M2" s="16">
+      <c r="N2" s="16">
         <v>1</v>
       </c>
-      <c r="N2" s="16">
+      <c r="O2" s="16">
         <v>10</v>
       </c>
-      <c r="O2" s="16">
+      <c r="P2" s="16">
         <v>20</v>
       </c>
-      <c r="P2" s="16">
+      <c r="Q2" s="16">
         <v>10</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>4</v>
       </c>
       <c r="R2" s="3">
         <v>4</v>
       </c>
       <c r="S2" s="3">
+        <v>4</v>
+      </c>
+      <c r="T2" s="3">
         <v>50</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="U2" s="18" t="s">
+      <c r="V2" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -942,9 +955,10 @@
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
-      <c r="U3" s="18"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U3" s="3"/>
+      <c r="V3" s="18"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -965,9 +979,10 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="18"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U4" s="3"/>
+      <c r="V4" s="18"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -988,9 +1003,10 @@
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
-      <c r="U5" s="18"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U5" s="3"/>
+      <c r="V5" s="18"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1011,111 +1027,123 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="19"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U6" s="1"/>
+      <c r="V6" s="19"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="U14" s="20"/>
-    </row>
-    <row r="15" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="V14" s="20"/>
+    </row>
+    <row r="15" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U15" s="20"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="V15" s="20"/>
+    </row>
+    <row r="16" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="V16" s="20"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-    </row>
-    <row r="18" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+    </row>
+    <row r="19" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="U18" s="20"/>
-    </row>
-    <row r="19" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
+      <c r="V19" s="20"/>
+    </row>
+    <row r="20" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="U19" s="20"/>
-    </row>
-    <row r="20" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21" t="s">
-        <v>69</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
-      <c r="U20" s="20"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="G20" s="21"/>
+      <c r="V20" s="20"/>
+    </row>
+    <row r="21" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="G21" s="21"/>
+      <c r="V21" s="20"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="22"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="B23" s="22"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A26" s="21" t="s">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A27" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Little easier way to calculate discount.
</commit_message>
<xml_diff>
--- a/docs/Products upload.xlsx
+++ b/docs/Products upload.xlsx
@@ -267,7 +267,7 @@
     <t>Discount Percent</t>
   </si>
   <si>
-    <t>Discount Percent: If this is filled, then item will be shown as sale item and price would be calculated as (Amount - discount%) + VAT%, i.e. in Above case, (100 - 20) + 16.8 = 96.8 euros</t>
+    <t>Discount Percent: If this is filled, then item will be shown as sale item and price would be calculated as (Amount - discount%) + VAT%, i.e. in Above case, (100 - 20) x 1.21 = 96.8 euros</t>
   </si>
 </sst>
 </file>
@@ -769,7 +769,7 @@
   <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Products upload excel sheet: updated rings_subcategory, material table, added discount column.
</commit_message>
<xml_diff>
--- a/docs/Products upload.xlsx
+++ b/docs/Products upload.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="48" windowWidth="16260" windowHeight="6888" tabRatio="491"/>
+    <workbookView xWindow="384" yWindow="48" windowWidth="16260" windowHeight="6888" tabRatio="491" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
   <si>
     <t>Company Id</t>
   </si>
@@ -249,15 +249,6 @@
     <t>Images: comma "," separated images link</t>
   </si>
   <si>
-    <t>Half Eternity Ring</t>
-  </si>
-  <si>
-    <t>Full Eternity Ring</t>
-  </si>
-  <si>
-    <t>Solitaire Ring</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -268,6 +259,27 @@
   </si>
   <si>
     <t>Discount Percent: If this is filled, then item will be shown as sale item and price would be calculated as (Amount - discount%) + VAT%, i.e. in Above case, (100 - 20) x 1.21 = 96.8 euros</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Platinum</t>
+  </si>
+  <si>
+    <t>Full Eternity Diamond Ring</t>
+  </si>
+  <si>
+    <t>Half Eternity Diamond Ring</t>
+  </si>
+  <si>
+    <t>Solitaire Diamond Ring</t>
+  </si>
+  <si>
+    <t>Gems Ring</t>
+  </si>
+  <si>
+    <t>Pearls Ring</t>
   </si>
 </sst>
 </file>
@@ -432,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -464,6 +476,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -768,7 +782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -812,10 +826,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
@@ -1053,13 +1067,13 @@
     </row>
     <row r="15" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="V15" s="20"/>
     </row>
     <row r="16" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="V16" s="20"/>
     </row>
@@ -1219,7 +1233,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -1231,18 +1245,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1255,11 +1269,27 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1503,30 +1533,30 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1535,7 +1565,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1543,15 +1573,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>78</v>
+      <c r="B5" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>